<commit_message>
file tree init by 이진규
</commit_message>
<xml_diff>
--- a/클래스설계서.VER.0.1.xlsx
+++ b/클래스설계서.VER.0.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Companion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AD5153-3351-4A21-97C4-6BCEFF93A89F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DF9EDA-4954-4DBF-8164-B8BB32016F7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{9F96F7B2-AB41-41A9-8B73-61A96A4507EF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>com.bit.companion</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -297,6 +297,22 @@
   </si>
   <si>
     <t>LoginServiceImpl.java</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이름</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>역할</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마감일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020.03.13</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -304,7 +320,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,10 +466,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -771,13 +787,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA3AAA0B-C88C-42AF-A0F4-6C7B93958BE6}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="A1:I29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.875" bestFit="1" customWidth="1"/>
@@ -790,7 +806,7 @@
     <col min="9" max="9" width="19.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -804,15 +820,24 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="1"/>
       <c r="G2" s="5" t="s">
         <v>25</v>
@@ -821,8 +846,11 @@
         <v>54</v>
       </c>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="L2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="3" t="s">
@@ -841,7 +869,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="3" t="s">
@@ -860,7 +888,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="3" t="s">
@@ -879,7 +907,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="3" t="s">
@@ -898,7 +926,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="3" t="s">
@@ -917,7 +945,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="3" t="s">
@@ -936,22 +964,22 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="8" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="3" t="s">
@@ -963,8 +991,8 @@
       <c r="E10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8" t="s">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -972,7 +1000,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="3" t="s">
@@ -984,8 +1012,8 @@
       <c r="E11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="3" t="s">
         <v>6</v>
       </c>
@@ -993,7 +1021,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="3" t="s">
@@ -1005,8 +1033,8 @@
       <c r="E12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1014,7 +1042,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="3" t="s">
@@ -1026,8 +1054,8 @@
       <c r="E13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="3" t="s">
         <v>8</v>
       </c>
@@ -1035,7 +1063,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="3" t="s">
@@ -1047,8 +1075,8 @@
       <c r="E14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
       <c r="H14" s="3" t="s">
         <v>9</v>
       </c>
@@ -1056,7 +1084,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="3" t="s">
@@ -1068,8 +1096,8 @@
       <c r="E15" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="3" t="s">
         <v>10</v>
       </c>
@@ -1077,7 +1105,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5" t="s">
@@ -1085,8 +1113,8 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="3" t="s">
         <v>60</v>
       </c>
@@ -1094,7 +1122,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1113,7 +1141,7 @@
       </c>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1132,7 +1160,7 @@
       </c>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1147,7 +1175,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1162,7 +1190,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1177,7 +1205,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1192,20 +1220,20 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="3" t="s">
@@ -1222,7 +1250,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="3" t="s">
@@ -1239,7 +1267,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="3" t="s">
@@ -1256,7 +1284,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="3" t="s">
@@ -1273,7 +1301,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="3" t="s">
@@ -1290,7 +1318,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="3" t="s">
@@ -1309,17 +1337,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:A29"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="B23:B29"/>
-    <mergeCell ref="B9:B22"/>
-    <mergeCell ref="B2:B8"/>
     <mergeCell ref="G2:G8"/>
     <mergeCell ref="C16:C22"/>
     <mergeCell ref="G10:G16"/>
     <mergeCell ref="F9:F16"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A1:A29"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B23:B29"/>
+    <mergeCell ref="B9:B22"/>
+    <mergeCell ref="B2:B8"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>